<commit_message>
Contributor 1 - ExampleData2
I have added 2 new columns (Height and BMI Status)
</commit_message>
<xml_diff>
--- a/data/raw_data/exampledata2.xlsx
+++ b/data/raw_data/exampledata2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11009"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C04835F9-E58C-CD49-BA03-12310C49A522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D79316D-DF1B-D84C-BD32-97B4234EC8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,17 +11,28 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Codebook" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>Height</t>
   </si>
@@ -60,6 +71,15 @@
   </si>
   <si>
     <t>BMI Status</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>Unhealthy</t>
   </si>
 </sst>
 </file>
@@ -389,7 +409,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -405,7 +425,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>12</v>
@@ -421,6 +441,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -432,6 +458,12 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="D3">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -443,6 +475,12 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -454,6 +492,12 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="D5">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -465,6 +509,12 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -476,6 +526,12 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -487,6 +543,12 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
+      <c r="D8">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -498,6 +560,12 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
+      <c r="D9">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -509,6 +577,12 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
+      <c r="D10">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -520,6 +594,12 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
+      <c r="D11">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -528,6 +608,12 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
+      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -539,6 +625,12 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
+      <c r="D13">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -550,6 +642,12 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -560,6 +658,12 @@
       </c>
       <c r="C15" t="s">
         <v>4</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>